<commit_message>
See sheet 2 - updated column assignments
There are more than just these columns in the final master file, but
they should all be clearly related!
</commit_message>
<xml_diff>
--- a/H1B_Visa_Data_Mapping.xlsx
+++ b/H1B_Visa_Data_Mapping.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5842b0d6efd6fbf/Columbia/Fall 2017/Capstone/capstone-goldman-sachs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="238" documentId="6B71D73448CDF898BC359B3CD13F7DACB7538036" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{8DF1BFCA-BAA9-440C-84BA-890EE7044F41}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6675" windowHeight="10230" xr2:uid="{49DBD784-9410-4812-B6A2-6D7308B44A7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6675" windowHeight="10230" activeTab="1" xr2:uid="{49DBD784-9410-4812-B6A2-6D7308B44A7C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Final List" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Final List'!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="301">
   <si>
     <t>Submitted_Date</t>
   </si>
@@ -820,16 +825,151 @@
   </si>
   <si>
     <t>2016 Layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original Certification Date for a Certified_Withdrawn application </t>
+  </si>
+  <si>
+    <t>ORIGINAL_CERT_DATE</t>
+  </si>
+  <si>
+    <t>WILLFUL_VIOLATOR</t>
+  </si>
+  <si>
+    <t>PW_UNIT_OF_PAY_2</t>
+  </si>
+  <si>
+    <t>Unit of pay in second location</t>
+  </si>
+  <si>
+    <t>RETURN_FAX</t>
+  </si>
+  <si>
+    <t>PROCESS_DATE</t>
+  </si>
+  <si>
+    <t>WITHDRAWN</t>
+  </si>
+  <si>
+    <t>WORKSITE_CITY_2</t>
+  </si>
+  <si>
+    <t>WORKSITE_STATE_2</t>
+  </si>
+  <si>
+    <t>PREVAILING_WAGE_2</t>
+  </si>
+  <si>
+    <t>PW_WAGE_SOURCE_2</t>
+  </si>
+  <si>
+    <t>PW_WAGE_SOURCE_OTHER_2</t>
+  </si>
+  <si>
+    <t>WAGE_RATE_OF_PAY_2</t>
+  </si>
+  <si>
+    <t>WAGE_UNIT_OF_PAY_2</t>
+  </si>
+  <si>
+    <t>MAX_RATE_2</t>
+  </si>
+  <si>
+    <t>PART_TIME_2</t>
+  </si>
+  <si>
+    <t>PART_TIME</t>
+  </si>
+  <si>
+    <t>MAX_RATE</t>
+  </si>
+  <si>
+    <t>CERTIFICATION_END_DATE</t>
+  </si>
+  <si>
+    <t>CERTIFICATION_START_DATE</t>
+  </si>
+  <si>
+    <t>CASE_NUMBER</t>
+  </si>
+  <si>
+    <t>EMPLOYER_ADDRESS</t>
+  </si>
+  <si>
+    <t>PW_SOURCE_YEAR</t>
+  </si>
+  <si>
+    <t>PW_SOURCE_OTHER</t>
+  </si>
+  <si>
+    <t>PW_SOURCE_YEAR_2</t>
+  </si>
+  <si>
+    <t>WAGE_RATE_OF_PAY_FROM</t>
+  </si>
+  <si>
+    <t>WAGE_RATE_OF_PAY_TO</t>
+  </si>
+  <si>
+    <t>Rate of pay offered to (max)</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Wages</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Classification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -842,21 +982,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -870,7 +1004,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -893,57 +1027,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1260,1890 +1439,1893 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBDD29F-5E65-49A1-B035-4F8F1EBB4AF9}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="H31" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.53125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="30" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="30" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="30" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.53125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="15" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.73046875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.265625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="30" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="30" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="30" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="N1" s="12"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="9" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="9" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="65.650000000000006" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="9" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="9" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="9" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="M14" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="9" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="9" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="9" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="M20" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="9" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L21" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="9" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="66" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="M22" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="9" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="1"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="7"/>
     </row>
     <row r="24" spans="1:14" ht="26.65" x14ac:dyDescent="0.45">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="9" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="M25" s="13" t="s">
+      <c r="M25" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="9" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="K26" s="13" t="s">
+      <c r="K26" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="9" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="I27" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="L27" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="M27" s="17" t="s">
+      <c r="M27" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="N27" s="7" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="L28" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="M28" s="17" t="s">
+      <c r="M28" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" s="9" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="I29" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="M29" s="17" t="s">
+      <c r="M29" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="9" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="K30" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="M30" s="17" t="s">
+      <c r="M30" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="N30" s="9" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="9" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="H35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="I35" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J35" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="K35" s="13"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="1"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="7"/>
     </row>
     <row r="36" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="K36" s="13"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="1"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="7"/>
     </row>
     <row r="37" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I37" s="11" t="s">
+      <c r="I37" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="J37" s="11" t="s">
+      <c r="J37" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="K37" s="13"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="1"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="7"/>
     </row>
     <row r="38" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="I38" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J38" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="K38" s="13"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="1"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="7"/>
     </row>
     <row r="39" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="I39" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J39" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="K39" s="13"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="1"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="7"/>
     </row>
     <row r="40" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="I40" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="K40" s="13"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="1"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="7"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="9" t="s">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H41" s="4" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
     </row>
     <row r="43" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11" t="s">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
     </row>
     <row r="44" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="9" t="s">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H44" s="9" t="s">
+      <c r="H44" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I44" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="K44" s="13" t="s">
+      <c r="K44" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="L44" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="M44" s="13" t="s">
+      <c r="M44" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="N44" s="5" t="s">
+      <c r="N44" s="9" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="I45" s="13" t="s">
+      <c r="I45" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="J45" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="K45" s="13"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="1"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="7"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="I46" s="13" t="s">
+      <c r="I46" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K46" s="13"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="1"/>
+      <c r="J46" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="7"/>
     </row>
     <row r="47" spans="1:14" ht="52.5" x14ac:dyDescent="0.45">
-      <c r="I47" s="13" t="s">
+      <c r="I47" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="J47" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="K47" s="17" t="s">
+      <c r="K47" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="L47" s="5" t="s">
+      <c r="L47" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="M47" s="17" t="s">
+      <c r="M47" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="N47" s="5" t="s">
+      <c r="N47" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K48" s="17" t="s">
+      <c r="K48" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="L48" s="5" t="s">
+      <c r="L48" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M48" s="17" t="s">
+      <c r="M48" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="N48" s="5" t="s">
+      <c r="N48" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="49" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K49" s="17" t="s">
+      <c r="K49" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="L49" s="5" t="s">
+      <c r="L49" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M49" s="17" t="s">
+      <c r="M49" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="N49" s="5" t="s">
+      <c r="N49" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="50" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K50" s="17" t="s">
+      <c r="K50" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="L50" s="5" t="s">
+      <c r="L50" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M50" s="17" t="s">
+      <c r="M50" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="N50" s="5" t="s">
+      <c r="N50" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="51" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K51" s="17" t="s">
+      <c r="K51" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="L51" s="5" t="s">
+      <c r="L51" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="M51" s="17" t="s">
+      <c r="M51" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="N51" s="5" t="s">
+      <c r="N51" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="52" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K52" s="17" t="s">
+      <c r="K52" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="L52" s="5" t="s">
+      <c r="L52" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="M52" s="17" t="s">
+      <c r="M52" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="N52" s="5" t="s">
+      <c r="N52" s="9" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="53" spans="11:14" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="K53" s="13" t="s">
+      <c r="K53" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="L53" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="M53" s="13" t="s">
+      <c r="M53" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="N53" s="1" t="s">
+      <c r="N53" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="54" spans="11:14" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="K54" s="13" t="s">
+      <c r="K54" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="L54" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="M54" s="13" t="s">
+      <c r="M54" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="N54" s="1" t="s">
+      <c r="N54" s="7" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="55" spans="11:14" x14ac:dyDescent="0.45">
-      <c r="K55" s="17" t="s">
+      <c r="K55" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="L55" s="5" t="s">
+      <c r="L55" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="M55" s="17" t="s">
+      <c r="M55" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="N55" s="5" t="s">
+      <c r="N55" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="56" spans="11:14" ht="52.5" x14ac:dyDescent="0.45">
-      <c r="K56" s="17" t="s">
+      <c r="K56" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="L56" s="5" t="s">
+      <c r="L56" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="M56" s="17" t="s">
+      <c r="M56" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="N56" s="5" t="s">
+      <c r="N56" s="9" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="57" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="L57" s="5" t="s">
+      <c r="L57" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="M57" s="13" t="s">
+      <c r="M57" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="N57" s="5" t="s">
+      <c r="N57" s="9" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="58" spans="11:14" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="K58" s="13" t="s">
+      <c r="K58" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="L58" s="5" t="s">
+      <c r="L58" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="M58" s="13" t="s">
+      <c r="M58" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="N58" s="5" t="s">
+      <c r="N58" s="9" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="59" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K59" s="13" t="s">
+      <c r="K59" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="L59" s="5" t="s">
+      <c r="L59" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="M59" s="13" t="s">
+      <c r="M59" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="N59" s="5" t="s">
+      <c r="N59" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="60" spans="11:14" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="K60" s="13" t="s">
+      <c r="K60" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="L60" s="5" t="s">
+      <c r="L60" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="M60" s="13" t="s">
+      <c r="M60" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="N60" s="5" t="s">
+      <c r="N60" s="9" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="61" spans="11:14" x14ac:dyDescent="0.45">
-      <c r="M61" s="2" t="s">
+      <c r="M61" s="10" t="s">
         <v>262</v>
       </c>
     </row>
@@ -3160,4 +3342,715 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DD48C3-D478-41C3-B251-76F5A121C882}">
+  <dimension ref="A1:C63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.265625" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="65.650000000000006" x14ac:dyDescent="0.45">
+      <c r="A6" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A15" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A16" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A17" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A18" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A19" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A20" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A21" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A25" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A26" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A28" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A29" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A33" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A34" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A35" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A37" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A40" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A41" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A42" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A43" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A44" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="26.65" x14ac:dyDescent="0.45">
+      <c r="A45" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A49" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A50" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A52" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A53" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="39.4" x14ac:dyDescent="0.45">
+      <c r="A54" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A56" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A57" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A58" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{4C377F90-F32A-4911-8706-33CBBD2CD69D}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>